<commit_message>
upgrade description in 外观检查.xlsx
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/外观检查 - 副本.xlsx
+++ b/AutoRegularInspection/外观检查 - 副本.xlsx
@@ -1,46 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1BB1A1-CDA9-4528-BA36-7B22559AF896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE5011-99A4-4FB8-80A4-458925455BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="7020" windowWidth="16815" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3825" windowWidth="28125" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
     <sheet name="上部结构" sheetId="2" r:id="rId2"/>
     <sheet name="下部结构" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+  <si>
+    <t>序号</t>
+  </si>
   <si>
     <t>位置</t>
   </si>
   <si>
-    <t>构件类型</t>
-  </si>
-  <si>
-    <t>损坏类型</t>
-  </si>
-  <si>
-    <t>病害描述</t>
-  </si>
-  <si>
     <t>图片描述</t>
   </si>
   <si>
@@ -59,7 +48,7 @@
     <t>左幅0#伸缩缝沉积物阻塞</t>
   </si>
   <si>
-    <t>166,168</t>
+    <t>855,858</t>
   </si>
   <si>
     <t>接缝处铺装碎边</t>
@@ -68,13 +57,16 @@
     <t>左幅0#伸缩缝接缝处铺装碎边</t>
   </si>
   <si>
+    <t>868</t>
+  </si>
+  <si>
     <t>右幅0#伸缩缝沉积物阻塞</t>
   </si>
   <si>
     <t>右幅1#伸缩缝沉积物阻塞</t>
   </si>
   <si>
-    <t>159,159,162,98</t>
+    <t>855,858,875</t>
   </si>
   <si>
     <t>栏杆</t>
@@ -86,9 +78,6 @@
     <t>从0#台起第8节栏杆缺失</t>
   </si>
   <si>
-    <t>171,173</t>
-  </si>
-  <si>
     <t>主梁</t>
   </si>
   <si>
@@ -98,15 +87,12 @@
     <t>左幅主梁</t>
   </si>
   <si>
-    <t>193</t>
+    <t>855</t>
   </si>
   <si>
     <t>右幅主梁</t>
   </si>
   <si>
-    <t>181</t>
-  </si>
-  <si>
     <t>0#台</t>
   </si>
   <si>
@@ -131,9 +117,15 @@
     <t>左幅1#台台身露筋锈蚀</t>
   </si>
   <si>
+    <t>858</t>
+  </si>
+  <si>
     <t>右幅1#台台身露筋锈蚀</t>
   </si>
   <si>
+    <t>875</t>
+  </si>
+  <si>
     <t>支座</t>
   </si>
   <si>
@@ -143,11 +135,15 @@
     <t>右幅支座完好</t>
   </si>
   <si>
-    <t>序号</t>
+    <t>要素</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>167</t>
+    <t>缺损类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺损描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -160,13 +156,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -262,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -297,7 +292,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -472,51 +467,44 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -524,22 +512,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -547,22 +535,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -570,19 +558,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -591,22 +579,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -614,22 +602,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -638,7 +626,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
@@ -646,7 +634,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
@@ -670,7 +658,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
@@ -696,49 +684,184 @@
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1501B7A2-AA81-40D9-9750-EC1FE7C158FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -746,22 +869,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -769,22 +892,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -837,47 +960,45 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29A3D48-2E34-4711-AE59-F4F03DE1DEC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -885,22 +1006,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="2">
-        <v>176</v>
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -908,22 +1029,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="2">
-        <v>182</v>
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -931,22 +1052,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="2">
-        <v>199</v>
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -954,22 +1075,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2">
-        <v>185</v>
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -977,22 +1098,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="2">
-        <v>209</v>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1000,26 +1121,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="2">
-        <v>189</v>
+        <v>36</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>